<commit_message>
update wishes. add wonder animation.
</commit_message>
<xml_diff>
--- a/assets/data/wishes.xlsx
+++ b/assets/data/wishes.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -255,6 +255,10 @@
   </si>
   <si>
     <t>Meat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attraction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -656,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -670,7 +674,7 @@
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -698,8 +702,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -727,8 +734,11 @@
       <c r="I2" s="1">
         <v>0.1</v>
       </c>
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -756,8 +766,11 @@
       <c r="I3" s="1">
         <v>0.1</v>
       </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -784,6 +797,9 @@
       </c>
       <c r="I4" s="1">
         <v>0.1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wheat and sun wish.
</commit_message>
<xml_diff>
--- a/assets/data/wishes.xlsx
+++ b/assets/data/wishes.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -246,19 +246,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Fire</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>attraction</t>
+    <t>Sun</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wheat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -660,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -703,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -743,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -755,7 +763,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -775,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -784,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -793,13 +801,77 @@
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1">
         <v>0.1</v>
       </c>
       <c r="J4" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>